<commit_message>
fix pie chart report and analisis
</commit_message>
<xml_diff>
--- a/keluhan_pembayaran_tiket.xlsx
+++ b/keluhan_pembayaran_tiket.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="217">
   <si>
     <t>content</t>
   </si>
@@ -28,15 +28,6 @@
     <t>kenapa pembayaran qris tidak bisa membayar tiket di kai acces,padahal saldo sudah di potong sesuai harga tiket,terhitung rugi uang,tolong respon nya</t>
   </si>
   <si>
-    <t>Aplikasinya sangat tidak competible. Saya melakukan pemesanan tiket PD ke PMN dengan PP berulang kali dikarenakan pembayaran tidak berhasil butuh dua hari untuk lebih untuk mendapatkan tiket online. Kode pembayaran tidak ada muncul hanya kode pemesanan saja. Dan metode pembayaran diprofil tidak ada gunanya diisi saat pesan tiket, pembayaran tiket hanya muncul duq metode saja ovo sm qris. Butuh pengembangan yg lebih baik lagi app nya karna tidak user friendly maupun competibel untuk app reservasi</t>
-  </si>
-  <si>
-    <t>Pelayanan aplikasi masih tidak jelas, saya top-up KAIpay untuk melakukan pembayaran tiket kereta yang di pesan lalu di minta untuk memasukan pin KAIpay sedangkan saat melakukan pendaftaran akun KAI-Access saya tidak di minta untuk membuat pin KAIpay, lalu bagaimana saya bisa memasukan pin KAIpay sedangkan saya tidak membuatnya? Terus saldo yang sudah saya top-up hangus begitu saja. Dasar manusia. Belum lagi saya mau hapus akun di minta kode OTP via SMS tapi tidak di kirim-kirim,</t>
-  </si>
-  <si>
-    <t>katanya pake KAI untuk mempermudah. tapi setiap mau payment tiket pake QRIS gagal, pake OVO gagal, mau dihubungkan pake debit mandiri lama verifikasinya wkwkw. tolong dong kalo gabisa melayani pembelian walk in aplikasinya diperbaiki biar pengguna nyaman.</t>
-  </si>
-  <si>
     <t>Jelek sekali pelayanan aplikasi ini. Biasanya pke link aja untuk membayar tiketnya tpi sudah gak ada dari daftar e walet,sudah isi link aja untuk beli tiket tpi sampah aplikasinya</t>
   </si>
   <si>
@@ -58,33 +49,18 @@
     <t>saya sudah bayar tiket lewat kai acces Saldo KaiPay berkurang tapi tiket tidak muncul. di hubungin cs belibet mulu BUMN kok kalah sama swasta, tolong aplikasi dan pelayanannya di tingkatkan, kecewa berat !!!!!</t>
   </si>
   <si>
-    <t>Audah melakukan pembayaran tiket dan pembayaran berhasil tapi e tiketnya tidak muncul di aplikasi. Padahal saldo di brimo juga sudah berkurang tapi tiketnya tidak muncul.</t>
-  </si>
-  <si>
     <t>Pas masih awal iy emang membantu tapi kenapa lama2 ini malah jadi merugikan ya. Saya udah bayar tiket tapi tiketnya tidak muncul malah disuruh melakukan pemesanan ulang. Kalau tiket gagal harusnya saldo kembali tapi kenapa malah saldo kepotong tapi tiketnya tidak muncul. Tolonglah min diperbaiki lagi ini sangat merugikan</t>
   </si>
   <si>
-    <t>Setelah update aplikasi, saldo KAIPay kembali. Hanya saja untuk pembayaran tiket dg KAIPay sempat terkendala, selain itu proses loading saat memilih kursi,pembayaran, lebih lama dari biasanya. Mohon diperbaiki kembali. Terima kasih.</t>
-  </si>
-  <si>
-    <t>App aneh..klo memang penumpang vaksinnya masih dosis satu,seharusnya waktu pembayaran tiketnya harusnya ditolak..tpi ini gk di tolak..uang pembayarannya di trima ma app ini..tp giliran penumpangnya mau masuk naik kreta di tolak ma petugas nya,dgn alasan dosis vaksinnya masih satu.. Dan aneh nya lagi pembatalan tiketny kena potongan...sungguh keterlaluan app ini... Jujur sy merasa di rugikan dgn aturan hal ini..</t>
-  </si>
-  <si>
     <t>Pakai KAIAccess dari jaman kuliah sampai sekarang udah kerja. Iseng-iseng aktivasi KAIPAY, udah ngisi saldo buat jaga-jaga kalau urgent beli tiket biar lebih gampang. Pas mau dipakai buat bayar tiket saldonya ilang. Kecewa banget</t>
   </si>
   <si>
-    <t>Aplikasinya lambat sekali. Beberapa kali terjadi eror pada sistem pembayaran tiketnya. Aplikasi perusahaan sebesar KAI butuh server yang besar juga.</t>
-  </si>
-  <si>
     <t>Aplikasi "yg kurang beradab / kurang manusiawi", masih merepotkan. Beli tiket sangat mudah kapan saja dan di mana saja. Pelunasan / bayar tiket juga mudah dari mana saja. Tapi refund &amp; reschedule tidak bisa dari aplilasi. Hmmmmm sistem yg arogan, maunya enak sendiri....</t>
   </si>
   <si>
     <t>Kode QR tidak bisa muncul walaupun sudah dicoba beberapa kali tetap tidak muncul jadi tidak bisa bayar tiketnya Lemot banget aplikasinya</t>
   </si>
   <si>
-    <t>Udah top up ke KAI Pay. Kemudian mau saya gunakan untuk pembayaran tiket,tapi gagal terus / error. Sampai sekarang masih ada saldo yang mengendap. 🥲🥲</t>
-  </si>
-  <si>
     <t>Sulit sekali mau bayar tiket nya, selalu stuck di tampilan menu. Mohon di perbaiki, ga bener banget sistem nya</t>
   </si>
   <si>
@@ -94,15 +70,9 @@
     <t>Saldo baru isi tgl 2,, tp skrng knp eror ya,, dr kemren gk bisa buat bayar tiket,,,, tolong jngan di persulit dong, jd gk bisa pulang kmpung minggu ini,,,</t>
   </si>
   <si>
-    <t>pembayaran tiket akan lebih baik jika ditambah e wallet nya jangan hanya satu, permudah juga untuk mengubah nomor hp nya</t>
-  </si>
-  <si>
     <t>Yg kasi bintang satu bilang aja lu gangerti pake aplikasi ini, BLOKKKK !!!! Skrg makin mudah kok bnayak alternatif lu pesan tiket atau bayar tiket, pelayanan bagus, bersih, manusiawi.</t>
   </si>
   <si>
-    <t>saya pribadi senang dengan UI yang baru ini, tidak monoton, elegan tapi tetap mengedepankan efisiensi, tidak berlebihan dari pemilihan font, warna, icon, homepage, dsb bagus. semoga kedepannya pembayaran tiket lokal bisa bekerja sama dengan banyak pihak, dapat di ubah kebijakannya tidak hanya eksklusif menggunakan aplikasi link aja.</t>
-  </si>
-  <si>
     <t>kok sistem pembayaran linkaja di hapus ya? padahal dah ngisi saldo pas mau bayar tiketnya ehhh malah gk ada sistem pambayaran linkaja nya malah diganti sama ovo</t>
   </si>
   <si>
@@ -124,18 +94,9 @@
     <t>Kecewa banget. Akun tidak bisa di update, salah masukin data yaudah salah selamanya... Trus pas pembayaran nggak ada menu lain selain "link aja". Yaudah nggak papa karena uda punya akun link aja, tp dengan nomor yg berbeda... ehh udah gitu no HPnya juga nggak bisa diganti... otomatis ga bisa bayar tiket karena link aja nya pakai nomor lain (bukan nomor yg terdaftar di kai access)... Tolong kalau belum siap untuk aplikasi nggak usah terbit dulu deh. Merepotkan dan bikin stress!</t>
   </si>
   <si>
-    <t>Tidak praktis, cara pembayaran tiket terbatas hanya bisa lewat link. Sistem sering offline padahal internet jalan, jadi susah pesan tiketnya. Masih butuh banyak perbaikan dalam tampilan applikasi dan kemudahan penggunaan.</t>
-  </si>
-  <si>
-    <t>Tolong diperbaiki metode pembayaran lewat kai pay (kaspro), jadi pas pembayaran tiket kereta selalu gagal karena kode pin salah, padahal saya sudah memasukkan kode nya dengan benar</t>
-  </si>
-  <si>
     <t>Banyak bug, udah bayar tiket tapi tidak muncul tiketnya Pdahal dari saldo jg sudah berkurang</t>
   </si>
   <si>
-    <t>Sistem buruk, saat akan melakukan pembayaran tiket lebaran pasti sangat mustahil untuk bisa</t>
-  </si>
-  <si>
     <t>Parah aplikasi selalu eror kl mau bayar tiket selalu balik lagi...!!!!!!!!!!!!!setelah itu tiket udah abis kehabisan tiket !!!</t>
   </si>
   <si>
@@ -157,21 +118,6 @@
     <t>aplikasi gak jelas, udah bayar tiket masih aja belum aktif tiketnya😡</t>
   </si>
   <si>
-    <t>tolong kalau bisa ditamabah untuk pembayaran lewat berbagai jenis ATM soalnya kalau pembayaran lewat link saja kurang nyaman karena aplikasi link sering bermasalah sekali lagi tolong ditambah untuk pembayaran tiket kereta api nya ditambah melewati semua jenis atm.terimakasih</t>
-  </si>
-  <si>
-    <t>Awalnya saya beri bintang 5 sekarang saya turunkan, sering eror di saat pembayaran,pembayaran tiket ka lokal lebih banyak dong pemilihan pembayarannya, jangan cuma link aja,ovo dan qris. sudah dibayar tapi kode tiket belum aktif dan akhirnya gagal,uang hangus dan pembatalan menunggu sampai 2 minggu juga tidak masuk ke saldo. Ayo perbaiki sistemnya perbanyak pilihan pembayaran di tiket ka lokal. Jangan sering eror. Thnks</t>
-  </si>
-  <si>
-    <t>masyarakat sebenarnya sangat perlu aplikasi ini. tapi masih banyak beberapa yang perlu di perbaiki, ex pusat bantuan alangkah baiknya di beri chat langsung saat ini masih email dan lama balasnya dan tidak adanya proses pembatalan pembayaran tiket..</t>
-  </si>
-  <si>
-    <t>Sangat membantu sih tapi untuk pembayaran tiket lokal pembayarannya ribet kurang banyak alternatif pmbayaran, harusnya di sediakan pembayaran dari indo/alfa juga biar enak, dan juga buat ganti nmr dan email lain susah harus ngajukan dulu ke emailnya dan gak langsung respond juga kok membuat customer bingung</t>
-  </si>
-  <si>
-    <t>Sangat membantu di saat sedang urgent tp tolong aplikasinya di perbarui lg agar calon penumpang Tidak dibuat kecewa akibat apknya lelet atau lemot pada saat mencari tiket dan pembayaran tiket dan juga pada saat calon penumpang ingin merubah jdwl keberangkatan agar TDK lemot dalam memprosesnya.</t>
-  </si>
-  <si>
     <t>Hbis update malah ga bisa dipakai.. mau bayar tiket malah qrisnya ga muncul, tpi keterngan tiketny menunggu.. gimana mau bayar kalo qrisnya ngga dapet? Seharusnya di kolom tiket yg menunggu itu di sediakan qrisnya biar ditampilkan, ini ngga ada.. terus mau bayar tikwtnya yg di scan apa? Menyusahkan</t>
   </si>
   <si>
@@ -187,63 +133,30 @@
     <t>Pada saat "Aktivasi KAI PAY" tidak ada prosedur untuk membuat PIN, akhirnya saya bisa melakukan top up saldo dengan harapan bisa lngsung digunakan untuk membayar tiket tapi pas mau bayar via KAI PAY di minta untuk memasukan PIN. Berpuluh-puluh kali dicoba untuk me-reset tapi aplikasi tidak bisa memunculkan kolom untuk merubah pin barunya, ini bagaimana ya dengan nasib saldo yang sudah di top up tapi tidak bisa digunakan?</t>
   </si>
   <si>
-    <t>Auto uninstall karena tiap pembayaran tiket pake Qris via gopay sering ga berhasil. Padahal sudah dapat notifikasi dari email kalau pembayaran berhasil tetapi ketika dicek di aplikasinya pembayaran belum terkonfirmasi. Alhasil tiket dan uang hangus. Tolong diperbaiki lagi kualitas layanan kedepannya.</t>
-  </si>
-  <si>
     <t>Bayar tiket melalui bca virtual account pada tgl 22 maret. saldo sudah ketarik tp tiket nya ga muncul. Bilang ke cs nya katanya time out saat pembayaran, padahal saat va keluar lgsg melakukan pembayaran. Katanya akan ditanyakan ke pihak terkait. Namun sampai sekarang blm ada info apa2. Apk udh bagus tolonglah pelayanannya jgn jelek2 amat</t>
   </si>
   <si>
     <t>Kecewa banget kenapa pas udah bayar tiketnya ngk muncul, padahal udah tepat waktu bayarnya. Udah 2 kali kayak gini, jadi mau ga mau harus beli lagi bayar dobel😪</t>
   </si>
   <si>
-    <t>saya melakukan pembayaran tiket via virtual acount bca sudah ke potong saldonya tp di notipikasi tiket di aplikasi kai nya masih belum di bayar sampai jadi kadaluarsa,sehingga harus booking lagi dan bayar lagi via indomaret karena trauma pake virtual acount,sudah komplent k cs kai di buatkan laporan, disuruh email bukti pembayaran yg sudah k debit,sudah di email tp tidak ada balesan(apa di proses??),bagai mna dg uang saya masa tidak balik lagi???</t>
-  </si>
-  <si>
     <t>KAIpay dalam perbaikan melulu, orang yang uangnya tertahan disitu jadi kesusahan akan berpergian karena tidak bisa membayar tiket, sangat disayangkan!</t>
   </si>
   <si>
     <t>Not recommended dah....... Tiap kali transaksi ga pernah bisa, udah bayar tiket nya ga berhasil ke booking padahal saldo udah kedebet. Aplikasi blank..Coba beberapa kali tetep sama. Payaaah bgt 👎👎👎</t>
   </si>
   <si>
-    <t>Zaman udh semakin maju,semua bisa di akses dr Gadget. Udh bagus sich aplikasi ini tp msh kurang sempurna Krn klo mau ubah jadwal/pembatalan gak bisa di akses utk KA LoKal msh harus DTG ke service center ke stasiun padahal tinggal nanti uang nya dikembalikan via alat pembayaran yg digunkan saat pembayaran tiket. Dan seharusnya sudah mencakup semua lah!!</t>
-  </si>
-  <si>
-    <t>Aplikasinya memang sanggat membantu dalam pemesanan ticket,tapi saran saya,metode pembayaran tiket kjj (kereta jarak jauh),harus disetarakan dengan metode pembayaran link aja.Agar lebih mudah dan praktis,untuk dalam pelayanan pembayaran ticket.</t>
-  </si>
-  <si>
-    <t>tidak ada option hapus akun, hanya bisa melakukan transaksi pembayaran tiket via link aja yang nomornya sesuai dengan akun kai, jadi jika akun link aja berbeda dengan nomor akun kai tidak bisa melkukan pembayaran tiket</t>
-  </si>
-  <si>
     <t>Sudah bayar tiket via kai access tapi kode bokingnya ga keluar. Sudah cek email berkali" tapi tapi ga ada email kode booking dari kai access. Menghubungi cs via email dan kirim bukti pembayaran tapi tidak ada respon. Nyeles banget order tiket disini</t>
   </si>
   <si>
     <t>Aplikasinya parah banget, giliran udah isi saldo link aja, buat bayar tiket kereta. Malah maintanance ga berhenti berhenti, Tolong dong Bagia IT nya jangan tidur Mulu. Maintanance Aplikasi ini mau sampe brapa lama dong?</t>
   </si>
   <si>
-    <t>Inovasi luar biasa dari KAI dengan adanya fitur terbaru tidak usah datang ke stasiun hanya untuk menjadwal ulang ataupun membatalkan tiket. Recommended banget buat yang suka traveling yang ingin tidak usah repot-repot pesan ke stasiun. Harapannya untuk aplikasi ini mohon ditambahkan metoda pembayaran tiket kereta api lokal. Terimakasih</t>
-  </si>
-  <si>
-    <t>Tolong dong. Tipe pembayaran tiket penataran/dhoho ditambah lagi. Biar lebih gampang. Saat ini saya pakai link aja, tapi tiap saya mau bayar tbtb log out gitu. Semoga segera diperbaiki yaa</t>
-  </si>
-  <si>
     <t>Sangat buruk. Sdh berhasil bayar tiket dg Link Aja tp e-tiket tdk muncul, dan kemudian oleh KAI Access malah dinyatakan hangus. Mau order jg sangat sering time out.</t>
   </si>
   <si>
-    <t>Knapa kok pembayaran tiket kereta pakai i-banking, tidak ada bank BCA, karna saya nasabah BCA. Dulu ada, tapi sekarang gak ada. Tiap bayar, harus ke indomaret. Menyusahkan. belom lagi kalo mau reschdule, harus pergi lagi ke indomaret buat bayar.</t>
-  </si>
-  <si>
-    <t>Mohon penjelasann dari pihak KAI Acces. Kenapa aplikasi KAI Acces selalu nge-close setiap setelah menerima sms kode OTP dalam proses pembayaran tiket via link aja? Saya pesan tiket ulang berkali-kali problem nya selalu sama.</t>
-  </si>
-  <si>
-    <t>Tolonglah kai acces , itu fungsi kaipay untuk apa , sy isi saldo agar permudah untuk pembayaran tiket , sudah pesan giliran mau bayar gak ada plihan untuk bayar melalui kai pay , sudah isi saldo . Mau tarik kembalipun ga bisa, sya coba isi pulsa pun gagal uang gak kembali ke kaipay . Tolong lah gmna cara tarik kmbali uang sya!!</t>
-  </si>
-  <si>
     <t>Selamat beraktivitas 🤗 saya mau tanya setelah saya beli tiket terus di direct ke LINK Aja tetapi gamuncul-muncul slip bayarnya, lalu saya back, terus masuk menu ticket --》 menunggu --》 kok gak bisa saya bayar ? Dan gak ada tombol apapun untuk bayar tiket.. tolong jawabannya pliss ❗❗❗❗❗</t>
   </si>
   <si>
-    <t>untuk Aplikasi sudah ok namun yang saya sayangkan dan kecewakan adalah untuk pembayaran Tiket KA Lokal ditambahilah opsinya jangan via LinkAja doang, giliran pembayaran via LinkAja untuk tiket KA lokal trobel bingung cara bayarnya. Atau disamakan dengan pembayaran tiket KA jarak jauh yang memudahkan masyarakat untuk bepergian dengan Kareta Api Semoga Feed Back ini bisa memperbaiki sistem app KAI Access. Sekian Terima Kasih</t>
-  </si>
-  <si>
     <t>Aplikasi ini sangat membantu menemukan jadwal keberangkatan kereta,cocok buat yang pengen simpel dalam memesan dan membayar tiket serta bisa memilih tempat duduk sendiri pokoknya saya sangat terbantu dengan aplikasi ini dan saran dari saya adalah supaya dibuatkan jadwal keberangkatan yang lebih detail lagi diluar jadwal yang ada pada kolom pesannan tiket</t>
   </si>
   <si>
@@ -253,39 +166,18 @@
     <t>aplikasi cacat, kalo aplikasi belom jadi jangan di publis dulu kek. masa saya udah mesen tiket, udah masuk riwayat pemesanan, status menunggu dikasih waktu bayar 15 menit, tapi gaada fitur untuk bayar tiket yg udah masuk riwayat menunggu, saya cari ke semua menu kaga ada pilihan untuk bayar tiketnya. bikin emosi aja</t>
   </si>
   <si>
-    <t>Kenapa akhir² ini saat pembayaran tiket tidak seperti biasanya ,tapi malah di redirect ke aplikasi link aja? Dan ujungnya selalu gagal melakukan pembayaran, tolong ditingkatkan lagi</t>
-  </si>
-  <si>
     <t>Kenapa harus hanya link saja untuk bayar tiket.. Dengan yang lain ga bissaaAa.. Kebijakan yang mempersulit.. Bahkan customer service pt kai pun bilang pin link salah padahal pin sudah benar dan bisa di ganti.. Kalau pun salah pin link ga bisa di ganti Jangan mempersulit rakyat</t>
   </si>
   <si>
-    <t>mohon untuk di perbaiki supaya pembayaran tiket ka lokal tidak hanya memakai linkaja tetapi bisa memakai cara cara yang lain seperti pembayaran tiket kereta api jarak jauh karena tidak semua orang memakai linkaja</t>
-  </si>
-  <si>
     <t>Gimana caranya melakukan pembayaran ulang pada pembayaran yg tertunda? Tidak ada tombol klik "Bayar" pada saat akan membayar tiket yg ter-pending pembayarannya.</t>
   </si>
   <si>
-    <t>Tolong untuk pembayaran tiket lokalnya ditambah ya... kalo bisa transfer bank langsung... ini saat mau bayar masukin kode verifikasinya keluar2 sendiri... jadi ga bisa pesen kalo gini tolong ya min</t>
-  </si>
-  <si>
-    <t>Knapa pembayaran tiket kreta api lokal sulit and ribet...knapa ndak ada pilihan lain yg lebih muda...pesan tiketnya mudah tingal bayarnya ribet mana sulit sekali masuknya.... Hmmm..</t>
-  </si>
-  <si>
     <t>Bayar tiket pakai Qris langsung bayar dan udah kepotong saldo tapi tiket ga keluar, mau beli tiket langsung di Stasiun Sepanjang tapi gabisa karna ga ada pelayannya. ANEH BGT. Akhirnya gabisa berangkat kerja.</t>
   </si>
   <si>
-    <t>Saya kasih bintang 4 dulu karena saya tidak tau cara pembayaran tiket KAI Access via tukarkan poin yang di kumpul dan semoga cepat di update lumayan sering lah saya beli tiket kereta api</t>
-  </si>
-  <si>
-    <t>Mohon untuk Metode pembayaran tiket KA loka, ditambahin lewat loket.. Karena pake aplikasi LinkAja, prosesnya terlalu ribet.. Mohon untuk PT. KAI dipermudah lagi buat pembayaran tiket Lokal..</t>
-  </si>
-  <si>
     <t>Min, kenapa pas saya mau bayar tiketnya cuma sampai rincian pemesanan saja pas mau pilih bayar skrang gak bisa di klik sama sekali, mohon sekali bantuannya min, karena aplikasi ini cukup membantu buat saya</t>
   </si>
   <si>
-    <t>Kenapa pembayaran tiket nya hanya lewat aplikasi LINK AJA? Apakah tidak ada cara bayar lainnya? Monopoli pmbayaran ini juga sangat menyulitkan. Karena tidak semua orang mempunyai aplikasi tersebut.</t>
-  </si>
-  <si>
     <t>Saldo sudah kepotong untuk membayar tiket, tapi tiket tidak muncul ( tidak terkonfirmasi ) padahal jelas dari Dana nya sudah terpotong, di tungguin sampai 14 hari kerja, ini sudah lebih dari 14 hari kerja siapa tau dananya masuk, ehh pas di cek setiap hari dari riwayat ngga ada saldo dana masuk. Kalo ngga bisa ngasih kepastian jangan bikin harapan dan balikin uang itu, ssusah nyarinya harus sanpe begadang demi mendapatkan uang. Parah sih udah lebih dari 14 hari ngga di balikin duitnya..</t>
   </si>
   <si>
@@ -304,9 +196,6 @@
     <t>Sebelum tak update, pas mau bayar tiket selalu otomatis kluar apknya, ni update yg tak tunggu2 akhirnya datang jg, skrng sdh lancar beli tiket lokal kai, thanks</t>
   </si>
   <si>
-    <t>Di proses pembayarannya kok gak bisa trus ya.. Padahal saldo di link aja sudah melebihi harga pembayaran tiket nya.</t>
-  </si>
-  <si>
     <t>Gak jelas banget aku udah bayar kereta lokal dari Blitar ke malang kok gak mau ya sama aku bayar tiket malang Banyuwangi kok gak bisa bisa pembayaran nya ribet beda sama Traveloka</t>
   </si>
   <si>
@@ -328,21 +217,12 @@
     <t>Kenapa boarding pass dan ID saya tidak keluar di tiket? padahal saya sudah membayar tiket lunas dan mengisi data dengan benar. Dan sebelum sebelumnya juga keluar boarding pass dan id saya.</t>
   </si>
   <si>
-    <t>tolong dong untuk pembayaran tiket ka lokal dipermudah, jangan lewat apk linkaja,. karena susah di akses untuk handphone yang terdeteksi root</t>
-  </si>
-  <si>
     <t>Untuk metode pembayaran dengan qris kadang eror/lama nunggu, setelah masuk aplikasi lagi untuk membayar tiket yg sudah dipesan tidak ada</t>
   </si>
   <si>
     <t>Saya sudah bayar tiket kereta. Saldo sudah berkurang tapi pemesanan gagal. Mencoba menghubungi email tapi tidak bisa. Bagaimana cara refund saldo!!</t>
   </si>
   <si>
-    <t>Kalo bikin aplikasi yg niat donk. Pembayaran tiket aja ruwet. Kasih pilihan alternatif kan banyak. Yg rancang kurang cerdas.</t>
-  </si>
-  <si>
-    <t>waktu pembayaran tiket pramek kenapa gagal terus yaa..padahal saldo LINKAJA masih ada..di ulang-ulang gagal terus waktu pembayaran.</t>
-  </si>
-  <si>
     <t>Sangat jelekkkkk.. sekarang semakin jelek aja, udah di update masih aja lambat. Pas bayar tiket habis terjual.</t>
   </si>
   <si>
@@ -364,45 +244,24 @@
     <t>Ya Allah emosi banget deh mau bayar tiket pake KaiPay. Pas masukin pin katanya data tidak ditemukan. Padahal pin nya bener loh. Udah ganti pin pun tetep aja gitu. Emosi banget woy lah. Terus uang di kaipay disuruh buat apa woy lah</t>
   </si>
   <si>
-    <t>Udah bayar pake shopeepay, tapi si tiket ga muncul trus, sampe waktu pembayaran tiketnya habis, mengecewakan.</t>
-  </si>
-  <si>
     <t>Untuk KA lokal, bayar tiketnya ribet. Mestinya bisa bayar pakai banyak pembayaran. Ga hanya link aj...</t>
   </si>
   <si>
-    <t>Kebijakan Aneh dari KAI. SANGAT BURUK Saat kita gagal berangkat, dan melakukan pembatalan tiket akibat faktor pribadi, unag pembayaran tiket tidak bisa dikembalikan saat pembatalan dan harus menunggu selama 30 hari. di samping itu harus dipotong 25%. Kalo dipotong sih wajar saja, tapi kalo disuruh nunggu 30 hari baru dikembalikan, itukan Kebijakan EDAN / GILA.</t>
-  </si>
-  <si>
-    <t>Kenapa ya pembayaran kok tidak bisa diproses, padahal di apk link aja udah terkonfirmasi pembayaran tiketnya. Tiketku malah hangus</t>
-  </si>
-  <si>
-    <t>aplikasi ini bagus hanya di hp lenovo a7000 di versi 5.0 selalu error di page pembayaran tiket kereta lokal memakai sitem bayar link aja, laporan juga sudah dikirim dgn lampiran log system hp saya. hp no root dan saldo ewallet 50.000 harga tiket 10.000. apa solusi yg admin KAI Access berikan ? tolong dijawab</t>
-  </si>
-  <si>
     <t>Sistem pembayaran nya error dan tidak ada refund. Masa bayar tiket 2 kali baru lancar. Kan gak masuk akal... Alim Rugi ???</t>
   </si>
   <si>
-    <t>Beberapa Hari Ini Aplikasi Sering Force Close Saat akan melakukan pembayaran Tiket , Diulang berkali kali juga sama Force Close saat akan pembayaran. Mohon diperbaiki aplikasi nya</t>
-  </si>
-  <si>
     <t>Min, nomer telp yg terdaftar di app ini salah, beda 1 angka dr nomor telp saya. Jadi saya tidak bs bayar pake linkAja. Mohon bantuannya supaya saya bisa membenahi no telp saya di app kai access. Urgent saya harus bayar tiket soalnya.</t>
   </si>
   <si>
     <t>Sudah jauh-jauh bayar tiket buat pergi ke alfa, sampai sana kode pemesanan tidak bisa.. nyesel pesen pakai aplikasi kai acces</t>
   </si>
   <si>
-    <t>Aplikasi yg sangat membantu untuk mempermudah pemesanan dan pembayaran tiket secara online... sudah tidak ribet lagi harus ke stasiun dengan ini...makin topcer saja🤩🤩🤩</t>
-  </si>
-  <si>
     <t>nyusahin app, app nya perlu perbaiki, seringnya buat rugi yang ngedownload, udah bayar tiket kereta tapi tiketnya ga ada nyusahin ni</t>
   </si>
   <si>
     <t>Parah si.. mau pulang, udah bayar tiket. Ga boleh masuk.. mohon uang bisa di kembalikan meski kena kelalaian sedikit, 20% atau berapa kek.. ini ga bisa di kembalikan</t>
   </si>
   <si>
-    <t>Mohon maaf ini aplikasinya banyak bugnya ya? Saya sudah melakukan pembayaran tiket ketika mau merubah jadwal kok tidak bisa?? Mohon kepada pengembang untuk diperbaiki</t>
-  </si>
-  <si>
     <t>aplikasi Ngebug Lag Saat Mau Cekout Tiket. Saya 4x mencoba Bayar tiket namun Gagal Terus. jadi Kursi Incaran Saya Tidak bisa saya dapatkan. SAAT PEMILIHAN KURSI JUGA SELALU BERHENTI. TIDAK GERAK SAMA SEKALI.</t>
   </si>
   <si>
@@ -412,27 +271,15 @@
     <t>bayar tiket masak harus pake aplikasi Link aja, gw mau bayar transfer gak ada pilihan nya. terlalu repot dan berbelit, pantes gak fleksibel kaya aplikasi swasta lain</t>
   </si>
   <si>
-    <t>Dalam pembayaran tiket online sebaiknya langsung menu bayar pake berbagai bank,biar cepat bisa diakses..</t>
-  </si>
-  <si>
     <t>Saya sudah bayar tiket tpi ngga muncul bukti tiketnya, uang sudah terlanjur kepotong&amp; gaada cara buat mengembalikn dana</t>
   </si>
   <si>
-    <t>Pelayanan masyarakat yang ribet proses pembayaran tiket skarang juga ribet harus dfatar akun link dll 👎 lebih enak pakek aplikasi lain banyak pilihan metode pembayaran ga kayak aplikasi ini 👎👎👎👎👎👎👎👎👎👎👎👎👎👎</t>
-  </si>
-  <si>
-    <t>Mengapa saat pembayaran tiket kai PIN Linkaja selalu salah padahal udah pernah buat cash ff dengan pin yang sama ternyata bisa mengapa buat kai acces tidak bisa tolong penjelasannya</t>
-  </si>
-  <si>
     <t>Tolong ganti metode pembayar tiket train lokal dengan OVO saja karna lebih mudah dan simple daripada LinkAja sering eror dan banyak komplain.</t>
   </si>
   <si>
     <t>Tiap log in invalid token, udh pesen udh bayar tiket ga muncul, ini selain pake apk ini ada ga sih yg bisa book ka lokal?</t>
   </si>
   <si>
-    <t>saya sudah melakukan pembayaran tiket dan saldo saya sudah terpotong tapi di aplikasi tertera masih menunggu pembayaran</t>
-  </si>
-  <si>
     <t>Aplikasi lemot , bnyk bugnya, padahal urgent banget fakfak, aplikasi burik ngelag lemot lama, apk penipuan udh bayar tiketnya ga muncul, gausa ada apk klo rusak kaya gni mah ngerugiin orng</t>
   </si>
   <si>
@@ -442,33 +289,18 @@
     <t>kesel banget udah refresh beberapa kali padahal udah bayar tiketnya tapi tiket pesanannya ngga ada di riwayat pesanan mana udah bayar lagi😒😒</t>
   </si>
   <si>
-    <t>Tolong perbaiki metode pembayaran tiket karna pada menu pembayaran yang tercantum hanya E-Wallet tidak ada pilihan lain atau retail pembayaran.</t>
-  </si>
-  <si>
     <t>Saya sudah melakukan pembayaran tiket via qris shopeepay. Tetapi setelah dibayar tiket tidak muncul🤬</t>
   </si>
   <si>
-    <t>susah bgt sih pas pembayaran tiket pke krtu kredit gagal2 trus klo cpet2an gk kyk tahun kmrn, tolong donk bgian pmbayaran krtu kredit bisa di smpan jdi gk perlu ngisi2 data2/nomer krtu kreditnya biar ngurangin wktu pmesanan tiket lebaran,</t>
-  </si>
-  <si>
     <t>Ini gimana ya kak!!!!! Saya udah membayar tiket tapi kok tiket nya hangus?? Dan saya tanyakan ke pihak stasiun, pihak stasiun tidak tau!!! Tolong kerjasamanya!!</t>
   </si>
   <si>
-    <t>Ubah nomor hp g bisa.. Pembayaran tiket KA lokal hanya lwat linkaja &amp; QRIS cb bisa pake internet banking pasti lbih mudah..</t>
-  </si>
-  <si>
-    <t>apa itu e wallet ..?? proses pembayaran tiket nya susah..tolong di perbaiki donk</t>
-  </si>
-  <si>
     <t>Aplikasi nya cacat pooolll. Masak udah bayar tiket via dana eh tiket nya gak muncul di KAI acces nya. Tolong sarannya min</t>
   </si>
   <si>
     <t>kaipay tidak bisa untuk membayar tiket</t>
   </si>
   <si>
-    <t>Metode pembayaran kok hanya debit mandiri, Adakah solusi pembayaran tiket dengan e wallet LinkAja?</t>
-  </si>
-  <si>
     <t>Sementara bintang satu dulu ya, ntar klo dah dapat tiket baru bintang lima. Susah pesan login dan bayar tiket</t>
   </si>
   <si>
@@ -478,39 +310,18 @@
     <t>Mau bayar tiket yg sudah di booking aja susahnya setengah mati. Padahal sudah download linkaja tapi tetep disuruh download.</t>
   </si>
   <si>
-    <t>Apakah pembayaran tiket online nya bisa mengunakan linkaja? Soalnya waktu tahun 2019 saldo linkaja bisa kenapa sekarang nggal bisa?</t>
-  </si>
-  <si>
     <t>Wkwkwkwk sangat lucu, saya sudah beli tiket + bayar tiket tp tiket itu hilang, joss boss ku... Terimakasih KAI sudah membuat saya kecewa😘</t>
   </si>
   <si>
-    <t>Sering keluar saat pembayaran tiket dilakukan, padahal lagi butuh 👍</t>
-  </si>
-  <si>
-    <t>untuk pembayaran tiketnya bagaimana? kenapa hanya ada pilihan e-wallet? trus cara top up nya bagaimana?</t>
-  </si>
-  <si>
     <t>Wahhh gabener nih apk udah bayar tiket, saldo berkurang tapi tiket gakebeli anj emang</t>
   </si>
   <si>
     <t>Tidak bisa bayar tiket karena nomer telp link aja dengan nomer telp kai berbeda dan tidak bisa di ganti dengan nomer telp link aja</t>
   </si>
   <si>
-    <t>sudah semakin baik pembaharuannya, semakin mudah melakukan pemesanan dan pembayaran tiket KAI sekarang</t>
-  </si>
-  <si>
-    <t>Pembayaran via link sdh dihapus dan skrg diganti via OVO..yg ga pny ovo harus download dl dan yg terlanjur pake apl.link ga berguna lg utk pembayaran tiket kenapa sih hrs digonta ganti,ribet bgt..</t>
-  </si>
-  <si>
     <t>Permisi, saya pengguna apk KAI ingin bertanya. Waktu teman saya login kai pembayaran tiket nya menggunakan akun link aja saya. Nah untuk sekarang dia sudah punya akun link aja sendiri tapi saat memesan tiket KAI pembayaran tetap di tagihkan ke akun link aja saya. Bagaimana cara mengganti pembayaran tersebut agar saat teman saya membayar tiket p KAI dia bisa menggunakan akun link aja nya sendiri ??  Terimakasih</t>
   </si>
   <si>
-    <t>Kenapa kok untuk pembayaran tiket sekrng tidak menggunakan link aja sih? Iya tidak semua orang punya kartu kredit.</t>
-  </si>
-  <si>
-    <t>server si uk terus saat pembayaran tiket..</t>
-  </si>
-  <si>
     <t>server ny kok sibuk terus. mau bayar tiket ga bisa bisa</t>
   </si>
   <si>
@@ -520,24 +331,9 @@
     <t>Aplikasi apaan masa gara" beda nomer aja ga bisa di bayar tiketnya hangus lah ini lah itu lah bikin repot aja aplikasi apaan ini</t>
   </si>
   <si>
-    <t>apakah pembayaran tiket lewat kai pay sudah tidak bisa di lakukan...? saya baru saja sudah aktivasi tapi tetap saja aktivasi lagi berkali kali . mohon bantuannya</t>
-  </si>
-  <si>
-    <t>tolong disediakan pembayaran tiket via m-banking dong... agar lebih simpel dan gk ribet</t>
-  </si>
-  <si>
     <t>Tolong dong pengembalian dana ko lama banget 30 hari gila aj, sudah 1bulan lebih g ad pemasukan sama sekali, PARAH bayar tiket mah harus buru2 bayar, giliran di batalin dana pembatalan di tunda sampe 30 hari</t>
   </si>
   <si>
-    <t>mudah dan aman serta fleksibel untuk pembayaran tiketnya.</t>
-  </si>
-  <si>
-    <t>Aplikasi mudah diakses n digunakan, alangkah LBH bagus jika sistem pembayaran tiket KA lokal juga bisa melalui transfer bank</t>
-  </si>
-  <si>
-    <t>Udah Lunas pembayaran tiket gag muncul di app, terus di suruh ke loket buat reprint 😒😒</t>
-  </si>
-  <si>
     <t>Memudahkan melihat jadwal kreta, tapi kok nga bisa bayar tiket pakai link aja ya, padahal seharusnya bisa, apa ada gangguan?</t>
   </si>
   <si>
@@ -547,21 +343,9 @@
     <t>Kenapa sekarang kl sy mau bayar tiketnya tertulis link/ovo pakai kai acces versi 4.9.8 punya sy masih versi 4.9.7</t>
   </si>
   <si>
-    <t>Tidak bisa payment tiket,ampe sekarang jadi beli tiket langsung :(</t>
-  </si>
-  <si>
     <t>2023-06-20 10:08:05</t>
   </si>
   <si>
-    <t>2023-04-22 11:07:25</t>
-  </si>
-  <si>
-    <t>2023-05-31 21:30:01</t>
-  </si>
-  <si>
-    <t>2023-05-19 20:43:46</t>
-  </si>
-  <si>
     <t>2023-04-17 00:07:31</t>
   </si>
   <si>
@@ -583,33 +367,18 @@
     <t>2023-03-05 04:19:30</t>
   </si>
   <si>
-    <t>2023-02-09 10:14:44</t>
-  </si>
-  <si>
     <t>2023-02-08 20:42:34</t>
   </si>
   <si>
-    <t>2023-02-21 11:28:56</t>
-  </si>
-  <si>
-    <t>2023-02-26 05:33:59</t>
-  </si>
-  <si>
     <t>2023-02-10 08:24:18</t>
   </si>
   <si>
-    <t>2023-02-07 08:19:55</t>
-  </si>
-  <si>
     <t>2023-05-04 11:01:18</t>
   </si>
   <si>
     <t>2023-02-05 10:15:08</t>
   </si>
   <si>
-    <t>2023-02-11 06:25:40</t>
-  </si>
-  <si>
     <t>2023-02-01 22:23:30</t>
   </si>
   <si>
@@ -619,15 +388,9 @@
     <t>2023-02-08 01:12:38</t>
   </si>
   <si>
-    <t>2023-05-04 20:07:41</t>
-  </si>
-  <si>
     <t>2023-05-02 19:00:35</t>
   </si>
   <si>
-    <t>2019-11-27 21:17:58</t>
-  </si>
-  <si>
     <t>2023-04-18 19:42:08</t>
   </si>
   <si>
@@ -649,18 +412,9 @@
     <t>2019-12-16 13:40:42</t>
   </si>
   <si>
-    <t>2019-10-20 18:22:41</t>
-  </si>
-  <si>
-    <t>2023-06-29 21:17:36</t>
-  </si>
-  <si>
     <t>2023-02-28 17:47:41</t>
   </si>
   <si>
-    <t>2023-03-15 00:17:03</t>
-  </si>
-  <si>
     <t>2023-03-07 01:00:14</t>
   </si>
   <si>
@@ -682,21 +436,6 @@
     <t>2023-02-05 22:00:12</t>
   </si>
   <si>
-    <t>2019-08-04 15:40:53</t>
-  </si>
-  <si>
-    <t>2022-07-05 19:13:43</t>
-  </si>
-  <si>
-    <t>2022-04-28 16:54:42</t>
-  </si>
-  <si>
-    <t>2022-07-04 15:01:13</t>
-  </si>
-  <si>
-    <t>2022-08-14 17:48:54</t>
-  </si>
-  <si>
     <t>2023-01-31 12:22:30</t>
   </si>
   <si>
@@ -712,63 +451,30 @@
     <t>2022-11-12 11:41:52</t>
   </si>
   <si>
-    <t>2022-04-04 20:41:07</t>
-  </si>
-  <si>
     <t>2022-03-27 14:34:04</t>
   </si>
   <si>
     <t>2023-02-13 19:24:56</t>
   </si>
   <si>
-    <t>2022-03-27 20:04:05</t>
-  </si>
-  <si>
     <t>2023-02-08 10:31:08</t>
   </si>
   <si>
     <t>2020-10-03 11:29:24</t>
   </si>
   <si>
-    <t>2022-03-12 13:48:05</t>
-  </si>
-  <si>
-    <t>2020-02-07 22:27:39</t>
-  </si>
-  <si>
-    <t>2020-02-16 07:58:11</t>
-  </si>
-  <si>
     <t>2018-11-13 15:11:27</t>
   </si>
   <si>
     <t>2020-03-17 11:08:32</t>
   </si>
   <si>
-    <t>2019-02-01 15:33:48</t>
-  </si>
-  <si>
-    <t>2019-03-03 15:38:49</t>
-  </si>
-  <si>
     <t>2020-02-21 14:06:13</t>
   </si>
   <si>
-    <t>2021-05-23 12:05:27</t>
-  </si>
-  <si>
-    <t>2019-09-14 22:11:52</t>
-  </si>
-  <si>
-    <t>2022-01-27 08:34:53</t>
-  </si>
-  <si>
     <t>2021-04-17 21:23:48</t>
   </si>
   <si>
-    <t>2020-01-12 13:54:03</t>
-  </si>
-  <si>
     <t>2022-03-15 21:31:19</t>
   </si>
   <si>
@@ -778,39 +484,18 @@
     <t>2022-08-14 08:14:40</t>
   </si>
   <si>
-    <t>2020-06-02 10:12:36</t>
-  </si>
-  <si>
     <t>2020-01-04 19:43:51</t>
   </si>
   <si>
-    <t>2019-05-26 16:10:55</t>
-  </si>
-  <si>
     <t>2020-02-09 17:06:40</t>
   </si>
   <si>
-    <t>2019-03-06 08:21:56</t>
-  </si>
-  <si>
-    <t>2019-08-31 15:29:44</t>
-  </si>
-  <si>
     <t>2022-08-09 08:01:26</t>
   </si>
   <si>
-    <t>2022-06-14 20:27:50</t>
-  </si>
-  <si>
-    <t>2019-11-28 11:39:27</t>
-  </si>
-  <si>
     <t>2021-06-19 00:05:26</t>
   </si>
   <si>
-    <t>2019-12-28 16:24:24</t>
-  </si>
-  <si>
     <t>2023-01-20 17:44:42</t>
   </si>
   <si>
@@ -829,9 +514,6 @@
     <t>2019-03-09 14:13:35</t>
   </si>
   <si>
-    <t>2019-11-26 15:48:02</t>
-  </si>
-  <si>
     <t>2022-09-17 15:01:34</t>
   </si>
   <si>
@@ -853,21 +535,12 @@
     <t>2020-11-30 19:27:17</t>
   </si>
   <si>
-    <t>2019-04-09 05:02:40</t>
-  </si>
-  <si>
     <t>2023-03-14 10:10:27</t>
   </si>
   <si>
     <t>2022-10-21 09:14:37</t>
   </si>
   <si>
-    <t>2019-12-18 20:46:22</t>
-  </si>
-  <si>
-    <t>2019-02-25 16:12:06</t>
-  </si>
-  <si>
     <t>2023-03-05 00:24:35</t>
   </si>
   <si>
@@ -889,45 +562,24 @@
     <t>2023-06-02 21:00:46</t>
   </si>
   <si>
-    <t>2021-10-14 14:59:06</t>
-  </si>
-  <si>
     <t>2020-07-18 11:21:57</t>
   </si>
   <si>
-    <t>2021-12-12 16:20:34</t>
-  </si>
-  <si>
-    <t>2020-08-02 22:38:12</t>
-  </si>
-  <si>
-    <t>2019-03-25 15:44:30</t>
-  </si>
-  <si>
     <t>2022-08-02 13:11:03</t>
   </si>
   <si>
-    <t>2021-11-27 08:59:18</t>
-  </si>
-  <si>
     <t>2020-03-12 15:51:16</t>
   </si>
   <si>
     <t>2019-11-27 21:11:03</t>
   </si>
   <si>
-    <t>2020-09-16 17:41:02</t>
-  </si>
-  <si>
     <t>2023-01-06 13:59:04</t>
   </si>
   <si>
     <t>2022-11-23 14:18:44</t>
   </si>
   <si>
-    <t>2022-05-13 15:11:18</t>
-  </si>
-  <si>
     <t>2021-06-30 06:41:39</t>
   </si>
   <si>
@@ -937,27 +589,15 @@
     <t>2019-03-15 16:46:56</t>
   </si>
   <si>
-    <t>2020-02-09 21:31:48</t>
-  </si>
-  <si>
     <t>2023-01-20 05:55:50</t>
   </si>
   <si>
-    <t>2020-03-04 22:26:54</t>
-  </si>
-  <si>
-    <t>2019-10-07 08:25:14</t>
-  </si>
-  <si>
     <t>2019-10-19 11:56:30</t>
   </si>
   <si>
     <t>2021-10-08 14:35:23</t>
   </si>
   <si>
-    <t>2022-10-08 03:23:36</t>
-  </si>
-  <si>
     <t>2022-12-16 14:06:56</t>
   </si>
   <si>
@@ -967,33 +607,18 @@
     <t>2022-07-13 22:23:34</t>
   </si>
   <si>
-    <t>2019-10-04 22:43:32</t>
-  </si>
-  <si>
     <t>2021-10-05 18:42:52</t>
   </si>
   <si>
-    <t>2019-03-12 00:12:52</t>
-  </si>
-  <si>
     <t>2020-12-22 18:04:49</t>
   </si>
   <si>
-    <t>2021-04-08 16:21:23</t>
-  </si>
-  <si>
-    <t>2019-07-02 20:09:21</t>
-  </si>
-  <si>
     <t>2022-07-13 22:15:48</t>
   </si>
   <si>
     <t>2023-03-21 10:31:52</t>
   </si>
   <si>
-    <t>2021-05-19 19:31:16</t>
-  </si>
-  <si>
     <t>2023-06-21 18:33:11</t>
   </si>
   <si>
@@ -1003,39 +628,18 @@
     <t>2020-07-05 08:41:53</t>
   </si>
   <si>
-    <t>2021-06-21 11:26:27</t>
-  </si>
-  <si>
     <t>2019-12-23 04:59:19</t>
   </si>
   <si>
-    <t>2022-06-08 08:00:24</t>
-  </si>
-  <si>
-    <t>2019-04-27 15:24:34</t>
-  </si>
-  <si>
     <t>2023-01-22 23:26:55</t>
   </si>
   <si>
     <t>2019-12-04 22:13:48</t>
   </si>
   <si>
-    <t>2021-06-11 14:06:36</t>
-  </si>
-  <si>
-    <t>2022-09-18 00:24:09</t>
-  </si>
-  <si>
     <t>2019-09-08 21:30:40</t>
   </si>
   <si>
-    <t>2020-02-05 06:34:48</t>
-  </si>
-  <si>
-    <t>2019-08-13 08:08:35</t>
-  </si>
-  <si>
     <t>2019-03-04 08:06:34</t>
   </si>
   <si>
@@ -1045,24 +649,9 @@
     <t>2020-02-02 22:31:03</t>
   </si>
   <si>
-    <t>2023-02-10 11:40:53</t>
-  </si>
-  <si>
-    <t>2018-12-31 11:15:24</t>
-  </si>
-  <si>
     <t>2020-04-23 06:56:36</t>
   </si>
   <si>
-    <t>2019-03-01 23:24:12</t>
-  </si>
-  <si>
-    <t>2021-10-02 17:38:03</t>
-  </si>
-  <si>
-    <t>2019-11-13 18:22:58</t>
-  </si>
-  <si>
     <t>2020-04-27 03:04:32</t>
   </si>
   <si>
@@ -1070,9 +659,6 @@
   </si>
   <si>
     <t>2022-05-31 17:10:14</t>
-  </si>
-  <si>
-    <t>2022-09-15 06:33:55</t>
   </si>
   <si>
     <t>Negative</t>
@@ -1436,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1458,10 +1044,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1469,10 +1055,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1480,10 +1066,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1491,10 +1077,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1502,10 +1088,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1513,10 +1099,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1524,10 +1110,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1535,10 +1121,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1546,10 +1132,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1557,10 +1143,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1568,10 +1154,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1579,10 +1165,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1590,10 +1176,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1601,10 +1187,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1612,10 +1198,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1623,10 +1209,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>193</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1634,10 +1220,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1645,10 +1231,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1656,10 +1242,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1667,10 +1253,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>197</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1678,10 +1264,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>198</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1689,10 +1275,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>199</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1700,10 +1286,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1711,10 +1297,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1722,10 +1308,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1733,10 +1319,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1744,10 +1330,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1755,10 +1341,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>205</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1766,10 +1352,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>206</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1777,10 +1363,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1788,10 +1374,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1799,10 +1385,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="C33" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1810,10 +1396,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="C34" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1821,10 +1407,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1832,10 +1418,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1843,10 +1429,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1854,10 +1440,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1865,10 +1451,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1876,10 +1462,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1887,10 +1473,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>217</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1898,10 +1484,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>218</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1909,10 +1495,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>219</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1920,10 +1506,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>220</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1931,10 +1517,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1942,10 +1528,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>222</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1953,10 +1539,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>223</v>
+        <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1964,10 +1550,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>224</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1975,10 +1561,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>225</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1986,10 +1572,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>226</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1997,10 +1583,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C51" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2008,10 +1594,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2019,10 +1605,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>229</v>
+        <v>160</v>
       </c>
       <c r="C53" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2030,10 +1616,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>230</v>
+        <v>161</v>
       </c>
       <c r="C54" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2041,10 +1627,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>231</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2052,10 +1638,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>232</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2063,10 +1649,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>233</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2074,10 +1660,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>234</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2085,10 +1671,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>235</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2096,10 +1682,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>236</v>
+        <v>167</v>
       </c>
       <c r="C60" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2107,10 +1693,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2118,10 +1704,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2129,10 +1715,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2140,10 +1726,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>240</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2151,10 +1737,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>241</v>
+        <v>172</v>
       </c>
       <c r="C65" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2162,10 +1748,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>242</v>
+        <v>173</v>
       </c>
       <c r="C66" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2173,10 +1759,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>174</v>
       </c>
       <c r="C67" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2184,10 +1770,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>244</v>
+        <v>175</v>
       </c>
       <c r="C68" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2195,10 +1781,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>245</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2206,10 +1792,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>246</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2217,10 +1803,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
+        <v>178</v>
       </c>
       <c r="C71" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2228,10 +1814,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>248</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2239,10 +1825,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>249</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2250,10 +1836,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>250</v>
+        <v>181</v>
       </c>
       <c r="C74" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2261,10 +1847,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>251</v>
+        <v>182</v>
       </c>
       <c r="C75" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2272,10 +1858,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>252</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2283,10 +1869,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>253</v>
+        <v>184</v>
       </c>
       <c r="C77" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2294,10 +1880,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>254</v>
+        <v>185</v>
       </c>
       <c r="C78" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2305,10 +1891,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>186</v>
       </c>
       <c r="C79" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2316,10 +1902,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>256</v>
+        <v>187</v>
       </c>
       <c r="C80" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2327,10 +1913,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>257</v>
+        <v>188</v>
       </c>
       <c r="C81" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2338,10 +1924,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>189</v>
       </c>
       <c r="C82" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2349,10 +1935,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>190</v>
       </c>
       <c r="C83" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2360,10 +1946,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>191</v>
       </c>
       <c r="C84" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2371,10 +1957,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>192</v>
       </c>
       <c r="C85" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2382,10 +1968,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2393,10 +1979,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>194</v>
       </c>
       <c r="C87" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2404,10 +1990,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>264</v>
+        <v>195</v>
       </c>
       <c r="C88" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2415,10 +2001,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>265</v>
+        <v>196</v>
       </c>
       <c r="C89" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2426,10 +2012,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>266</v>
+        <v>197</v>
       </c>
       <c r="C90" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2437,10 +2023,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>267</v>
+        <v>198</v>
       </c>
       <c r="C91" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2448,10 +2034,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>268</v>
+        <v>199</v>
       </c>
       <c r="C92" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2459,10 +2045,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>269</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2470,10 +2056,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="C94" t="s">
-        <v>354</v>
+        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2481,10 +2067,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="C95" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2492,10 +2078,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>272</v>
+        <v>203</v>
       </c>
       <c r="C96" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2503,10 +2089,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>273</v>
+        <v>204</v>
       </c>
       <c r="C97" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2514,10 +2100,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>274</v>
+        <v>205</v>
       </c>
       <c r="C98" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2525,10 +2111,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>275</v>
+        <v>206</v>
       </c>
       <c r="C99" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2536,10 +2122,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="C100" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2547,10 +2133,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C101" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2558,10 +2144,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>278</v>
+        <v>209</v>
       </c>
       <c r="C102" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2569,10 +2155,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>279</v>
+        <v>210</v>
       </c>
       <c r="C103" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2580,10 +2166,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>280</v>
+        <v>211</v>
       </c>
       <c r="C104" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2591,10 +2177,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>281</v>
+        <v>212</v>
       </c>
       <c r="C105" t="s">
-        <v>353</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2602,10 +2188,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
       <c r="C106" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2613,769 +2199,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>283</v>
+        <v>214</v>
       </c>
       <c r="C107" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>109</v>
-      </c>
-      <c r="B108" t="s">
-        <v>284</v>
-      </c>
-      <c r="C108" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>110</v>
-      </c>
-      <c r="B109" t="s">
-        <v>285</v>
-      </c>
-      <c r="C109" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>111</v>
-      </c>
-      <c r="B110" t="s">
-        <v>286</v>
-      </c>
-      <c r="C110" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>112</v>
-      </c>
-      <c r="B111" t="s">
-        <v>287</v>
-      </c>
-      <c r="C111" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>113</v>
-      </c>
-      <c r="B112" t="s">
-        <v>288</v>
-      </c>
-      <c r="C112" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113" t="s">
-        <v>289</v>
-      </c>
-      <c r="C113" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>115</v>
-      </c>
-      <c r="B114" t="s">
-        <v>290</v>
-      </c>
-      <c r="C114" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>116</v>
-      </c>
-      <c r="B115" t="s">
-        <v>291</v>
-      </c>
-      <c r="C115" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>117</v>
-      </c>
-      <c r="B116" t="s">
-        <v>292</v>
-      </c>
-      <c r="C116" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>118</v>
-      </c>
-      <c r="B117" t="s">
-        <v>293</v>
-      </c>
-      <c r="C117" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>119</v>
-      </c>
-      <c r="B118" t="s">
-        <v>294</v>
-      </c>
-      <c r="C118" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>120</v>
-      </c>
-      <c r="B119" t="s">
-        <v>295</v>
-      </c>
-      <c r="C119" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120" t="s">
-        <v>296</v>
-      </c>
-      <c r="C120" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>122</v>
-      </c>
-      <c r="B121" t="s">
-        <v>297</v>
-      </c>
-      <c r="C121" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>123</v>
-      </c>
-      <c r="B122" t="s">
-        <v>298</v>
-      </c>
-      <c r="C122" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>124</v>
-      </c>
-      <c r="B123" t="s">
-        <v>299</v>
-      </c>
-      <c r="C123" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>125</v>
-      </c>
-      <c r="B124" t="s">
-        <v>300</v>
-      </c>
-      <c r="C124" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>126</v>
-      </c>
-      <c r="B125" t="s">
-        <v>301</v>
-      </c>
-      <c r="C125" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
-        <v>127</v>
-      </c>
-      <c r="B126" t="s">
-        <v>302</v>
-      </c>
-      <c r="C126" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>128</v>
-      </c>
-      <c r="B127" t="s">
-        <v>303</v>
-      </c>
-      <c r="C127" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
-        <v>129</v>
-      </c>
-      <c r="B128" t="s">
-        <v>304</v>
-      </c>
-      <c r="C128" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" t="s">
-        <v>130</v>
-      </c>
-      <c r="B129" t="s">
-        <v>305</v>
-      </c>
-      <c r="C129" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" t="s">
-        <v>131</v>
-      </c>
-      <c r="B130" t="s">
-        <v>306</v>
-      </c>
-      <c r="C130" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>132</v>
-      </c>
-      <c r="B131" t="s">
-        <v>307</v>
-      </c>
-      <c r="C131" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" t="s">
-        <v>133</v>
-      </c>
-      <c r="B132" t="s">
-        <v>308</v>
-      </c>
-      <c r="C132" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" t="s">
-        <v>134</v>
-      </c>
-      <c r="B133" t="s">
-        <v>309</v>
-      </c>
-      <c r="C133" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>135</v>
-      </c>
-      <c r="B134" t="s">
-        <v>310</v>
-      </c>
-      <c r="C134" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" t="s">
-        <v>136</v>
-      </c>
-      <c r="B135" t="s">
-        <v>311</v>
-      </c>
-      <c r="C135" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" t="s">
-        <v>137</v>
-      </c>
-      <c r="B136" t="s">
-        <v>312</v>
-      </c>
-      <c r="C136" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" t="s">
-        <v>138</v>
-      </c>
-      <c r="B137" t="s">
-        <v>313</v>
-      </c>
-      <c r="C137" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138" t="s">
-        <v>139</v>
-      </c>
-      <c r="B138" t="s">
-        <v>314</v>
-      </c>
-      <c r="C138" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" t="s">
-        <v>140</v>
-      </c>
-      <c r="B139" t="s">
-        <v>315</v>
-      </c>
-      <c r="C139" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>141</v>
-      </c>
-      <c r="B140" t="s">
-        <v>316</v>
-      </c>
-      <c r="C140" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>142</v>
-      </c>
-      <c r="B141" t="s">
-        <v>317</v>
-      </c>
-      <c r="C141" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" t="s">
-        <v>143</v>
-      </c>
-      <c r="B142" t="s">
-        <v>318</v>
-      </c>
-      <c r="C142" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" t="s">
-        <v>144</v>
-      </c>
-      <c r="B143" t="s">
-        <v>319</v>
-      </c>
-      <c r="C143" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" t="s">
-        <v>145</v>
-      </c>
-      <c r="B144" t="s">
-        <v>320</v>
-      </c>
-      <c r="C144" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" t="s">
-        <v>146</v>
-      </c>
-      <c r="B145" t="s">
-        <v>321</v>
-      </c>
-      <c r="C145" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>147</v>
-      </c>
-      <c r="B146" t="s">
-        <v>322</v>
-      </c>
-      <c r="C146" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" t="s">
-        <v>148</v>
-      </c>
-      <c r="B147" t="s">
-        <v>323</v>
-      </c>
-      <c r="C147" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148" t="s">
-        <v>149</v>
-      </c>
-      <c r="B148" t="s">
-        <v>324</v>
-      </c>
-      <c r="C148" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" t="s">
-        <v>150</v>
-      </c>
-      <c r="B149" t="s">
-        <v>325</v>
-      </c>
-      <c r="C149" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" t="s">
-        <v>151</v>
-      </c>
-      <c r="B150" t="s">
-        <v>326</v>
-      </c>
-      <c r="C150" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" t="s">
-        <v>152</v>
-      </c>
-      <c r="B151" t="s">
-        <v>327</v>
-      </c>
-      <c r="C151" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" t="s">
-        <v>153</v>
-      </c>
-      <c r="B152" t="s">
-        <v>328</v>
-      </c>
-      <c r="C152" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" t="s">
-        <v>154</v>
-      </c>
-      <c r="B153" t="s">
-        <v>329</v>
-      </c>
-      <c r="C153" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" t="s">
-        <v>155</v>
-      </c>
-      <c r="B154" t="s">
-        <v>330</v>
-      </c>
-      <c r="C154" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" t="s">
-        <v>156</v>
-      </c>
-      <c r="B155" t="s">
-        <v>331</v>
-      </c>
-      <c r="C155" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" t="s">
-        <v>157</v>
-      </c>
-      <c r="B156" t="s">
-        <v>332</v>
-      </c>
-      <c r="C156" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" t="s">
-        <v>158</v>
-      </c>
-      <c r="B157" t="s">
-        <v>333</v>
-      </c>
-      <c r="C157" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158" t="s">
-        <v>159</v>
-      </c>
-      <c r="B158" t="s">
-        <v>334</v>
-      </c>
-      <c r="C158" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" t="s">
-        <v>160</v>
-      </c>
-      <c r="B159" t="s">
-        <v>335</v>
-      </c>
-      <c r="C159" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>161</v>
-      </c>
-      <c r="B160" t="s">
-        <v>336</v>
-      </c>
-      <c r="C160" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161" t="s">
-        <v>162</v>
-      </c>
-      <c r="B161" t="s">
-        <v>337</v>
-      </c>
-      <c r="C161" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" t="s">
-        <v>163</v>
-      </c>
-      <c r="B162" t="s">
-        <v>338</v>
-      </c>
-      <c r="C162" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" t="s">
-        <v>164</v>
-      </c>
-      <c r="B163" t="s">
-        <v>339</v>
-      </c>
-      <c r="C163" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" t="s">
-        <v>165</v>
-      </c>
-      <c r="B164" t="s">
-        <v>340</v>
-      </c>
-      <c r="C164" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
-      <c r="A165" t="s">
-        <v>166</v>
-      </c>
-      <c r="B165" t="s">
-        <v>341</v>
-      </c>
-      <c r="C165" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166" t="s">
-        <v>167</v>
-      </c>
-      <c r="B166" t="s">
-        <v>342</v>
-      </c>
-      <c r="C166" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" t="s">
-        <v>168</v>
-      </c>
-      <c r="B167" t="s">
-        <v>343</v>
-      </c>
-      <c r="C167" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168" t="s">
-        <v>169</v>
-      </c>
-      <c r="B168" t="s">
-        <v>344</v>
-      </c>
-      <c r="C168" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" t="s">
-        <v>170</v>
-      </c>
-      <c r="B169" t="s">
-        <v>345</v>
-      </c>
-      <c r="C169" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" t="s">
-        <v>171</v>
-      </c>
-      <c r="B170" t="s">
-        <v>346</v>
-      </c>
-      <c r="C170" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" t="s">
-        <v>172</v>
-      </c>
-      <c r="B171" t="s">
-        <v>347</v>
-      </c>
-      <c r="C171" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" t="s">
-        <v>173</v>
-      </c>
-      <c r="B172" t="s">
-        <v>348</v>
-      </c>
-      <c r="C172" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" t="s">
-        <v>174</v>
-      </c>
-      <c r="B173" t="s">
-        <v>349</v>
-      </c>
-      <c r="C173" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" t="s">
-        <v>175</v>
-      </c>
-      <c r="B174" t="s">
-        <v>350</v>
-      </c>
-      <c r="C174" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" t="s">
-        <v>176</v>
-      </c>
-      <c r="B175" t="s">
-        <v>351</v>
-      </c>
-      <c r="C175" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" t="s">
-        <v>177</v>
-      </c>
-      <c r="B176" t="s">
-        <v>352</v>
-      </c>
-      <c r="C176" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>